<commit_message>
Aanwezigheid en Planning edits
</commit_message>
<xml_diff>
--- a/Aanwezigheid/Aanwezigheid GL-G5.xlsx
+++ b/Aanwezigheid/Aanwezigheid GL-G5.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="56">
   <si>
     <t>Maandag</t>
   </si>
@@ -1094,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J76" sqref="J76"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,7 +1163,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="32">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B104+B112+B120+B128+B136+B144+B152+B168+B160+B176</f>
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="L2" s="47">
         <f>C8+C16+C24+C32+C48+C56+C64+C72+C80+C88+C96+C104+C120+C128+C136+C144+C152+C160+C168+C176</f>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="M2" s="53">
         <f>L2/K2</f>
-        <v>0.26315789473684209</v>
+        <v>0.25641025641025639</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>18</v>
@@ -1211,11 +1211,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="48">
         <f>D8+D16+D24+D32+D48+D56+D64+D72+D80+D88+D96+D104+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M3" s="54">
         <f>L3/K2</f>
-        <v>0.86842105263157898</v>
+        <v>0.87179487179487181</v>
       </c>
       <c r="N3" s="43" t="s">
         <v>19</v>
@@ -1253,11 +1253,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="49">
         <f>E8+E16+E24+E32+E48+E56+E64+E72+E80+E88+E96+E104+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="M4" s="55">
         <f>L4/K2</f>
-        <v>0.84210526315789469</v>
+        <v>0.84615384615384615</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>20</v>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="M5" s="56">
         <f>L5/K2</f>
-        <v>0.36184210526315791</v>
+        <v>0.35256410256410259</v>
       </c>
       <c r="N5" s="45" t="s">
         <v>21</v>
@@ -1337,11 +1337,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="51">
         <f>G8+G16+G24+G32+G48+G56+G64+G72+G80+G88+G96+G104+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M6" s="57">
         <f>L6/K2</f>
-        <v>0.80263157894736847</v>
+        <v>0.80769230769230771</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>22</v>
@@ -1379,11 +1379,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="52">
         <f>H8+H88+H24+H32+H48+H56+H64+H72+H80+H96+H104+H120+H128+H136+H144+H152+H160+H168+H176+H16</f>
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="M7" s="58">
         <f>L7/K2</f>
-        <v>0.81578947368421051</v>
+        <v>0.82051282051282048</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>23</v>
@@ -1428,11 +1428,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="38">
         <f>I8+I16+I24+I32+I48+I56+I64+I72+I80+I88+I96+I104+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="M8" s="39">
         <f>L8/K2</f>
-        <v>0.82894736842105265</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>24</v>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="M10" s="29">
         <f>SUM(M2:M9)</f>
-        <v>4.7828947368421053</v>
+        <v>4.7884615384615383</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3228,14 +3228,26 @@
       <c r="A83" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B83" s="10"/>
+      <c r="B83" s="10">
+        <v>4</v>
+      </c>
       <c r="C83" s="34"/>
-      <c r="D83" s="35"/>
-      <c r="E83" s="35"/>
+      <c r="D83" s="35">
+        <v>4</v>
+      </c>
+      <c r="E83" s="35">
+        <v>4</v>
+      </c>
       <c r="F83" s="35"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="35"/>
-      <c r="I83" s="36"/>
+      <c r="G83" s="35">
+        <v>4</v>
+      </c>
+      <c r="H83" s="35">
+        <v>4</v>
+      </c>
+      <c r="I83" s="36">
+        <v>4</v>
+      </c>
       <c r="J83" s="2"/>
       <c r="K83" s="10"/>
     </row>
@@ -3304,7 +3316,7 @@
         <v>5</v>
       </c>
       <c r="B88" s="32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C88" s="76">
         <f t="shared" ref="C88:G88" si="10">SUM(C83:C87)</f>
@@ -3312,11 +3324,11 @@
       </c>
       <c r="D88" s="77">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E88" s="77">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F88" s="77">
         <f t="shared" si="10"/>
@@ -3324,15 +3336,15 @@
       </c>
       <c r="G88" s="77">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H88" s="77">
         <f>SUM(H83:H87)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I88" s="78">
         <f>SUM(I83:I87)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J88" s="31"/>
     </row>

</xml_diff>

<commit_message>
A lot of work
Aanwezigheid, Planning en Presentatie werk
</commit_message>
<xml_diff>
--- a/Aanwezigheid/Aanwezigheid GL-G5.xlsx
+++ b/Aanwezigheid/Aanwezigheid GL-G5.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sepi\Documents\Important Portable Stuff V1\Year 2\Ninja Outbreak\Project-Ninja-Outbreak\Aanwezigheid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Important and Stuff V1\School\Year 2\Project-Ninja-Outbreak\Aanwezigheid\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="57">
   <si>
     <t>Maandag</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>David had Theorie examen / Hadewij en Walter ziek</t>
+  </si>
+  <si>
+    <t>David was ziek</t>
   </si>
 </sst>
 </file>
@@ -1094,23 +1097,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
-    <col min="3" max="9" width="10.88671875" style="84" customWidth="1"/>
-    <col min="10" max="10" width="37.6640625" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" style="84" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="22" t="s">
         <v>6</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1253,17 +1256,17 @@
       <c r="K4" s="10"/>
       <c r="L4" s="49">
         <f>E8+E16+E24+E32+E48+E56+E64+E72+E80+E88+E96+E104+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="M4" s="55">
         <f>L4/K2</f>
-        <v>0.81176470588235294</v>
+        <v>0.83529411764705885</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1337,17 +1340,17 @@
       <c r="K6" s="10"/>
       <c r="L6" s="51">
         <f>G8+G16+G24+G32+G48+G56+G64+G72+G80+G88+G96+G104+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M6" s="57">
         <f>L6/K2</f>
-        <v>0.77647058823529413</v>
+        <v>0.8</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1379,17 +1382,17 @@
       <c r="K7" s="10"/>
       <c r="L7" s="52">
         <f>H8+H88+H24+H32+H48+H56+H64+H72+H80+H96+H104+H120+H128+H136+H144+H152+H160+H168+H176+H16</f>
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="M7" s="58">
         <f>L7/K2</f>
-        <v>0.78823529411764703</v>
+        <v>0.81176470588235294</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1428,17 +1431,17 @@
       <c r="K8" s="10"/>
       <c r="L8" s="38">
         <f>I8+I16+I24+I32+I48+I56+I64+I72+I80+I88+I96+I104+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M8" s="39">
         <f>L8/K2</f>
-        <v>0.77647058823529413</v>
+        <v>0.8</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="79"/>
       <c r="D9" s="79"/>
       <c r="E9" s="79"/>
@@ -1448,7 +1451,7 @@
       <c r="I9" s="79"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="59" t="s">
         <v>26</v>
       </c>
@@ -1467,10 +1470,10 @@
       </c>
       <c r="M10" s="29">
         <f>SUM(M2:M9)</f>
-        <v>4.5470588235294116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4.6411764705882348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="60" t="s">
         <v>0</v>
       </c>
@@ -1501,7 +1504,7 @@
       <c r="J11" s="63"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>1</v>
       </c>
@@ -1538,7 +1541,7 @@
       </c>
       <c r="M12" s="87"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
         <v>2</v>
       </c>
@@ -1573,7 +1576,7 @@
       </c>
       <c r="M13" s="93"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
         <v>3</v>
       </c>
@@ -1608,7 +1611,7 @@
       </c>
       <c r="M14" s="94"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="61" t="s">
         <v>4</v>
       </c>
@@ -1645,7 +1648,7 @@
       </c>
       <c r="M15" s="95"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="61" t="s">
         <v>5</v>
       </c>
@@ -1687,7 +1690,7 @@
       </c>
       <c r="M16" s="96"/>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="79"/>
       <c r="D17" s="79"/>
       <c r="E17" s="79"/>
@@ -1698,7 +1701,7 @@
       <c r="J17" s="13"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1713,7 +1716,7 @@
       <c r="J18" s="62"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -1744,7 +1747,7 @@
       <c r="J19" s="63"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -1777,7 +1780,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1808,7 +1811,7 @@
       <c r="J21" s="63"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1841,7 +1844,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1875,7 @@
       <c r="J23" s="63"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -1910,7 +1913,7 @@
       <c r="J24" s="27"/>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="79"/>
       <c r="D25" s="79"/>
       <c r="E25" s="79"/>
@@ -1919,7 +1922,7 @@
       <c r="H25" s="79"/>
       <c r="I25" s="79"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
@@ -1934,7 +1937,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -1967,7 +1970,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
@@ -2000,7 +2003,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2015,7 +2018,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2046,7 +2049,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -2079,7 +2082,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
@@ -2117,7 +2120,7 @@
       <c r="J32" s="27"/>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="79"/>
       <c r="D33" s="79"/>
       <c r="E33" s="79"/>
@@ -2126,7 +2129,7 @@
       <c r="H33" s="79"/>
       <c r="I33" s="79"/>
     </row>
-    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
@@ -2143,7 +2146,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2177,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>1</v>
       </c>
@@ -2207,7 +2210,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -2240,7 +2243,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>3</v>
       </c>
@@ -2271,7 +2274,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>4</v>
       </c>
@@ -2304,7 +2307,7 @@
       </c>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>5</v>
       </c>
@@ -2341,10 +2344,10 @@
       </c>
       <c r="J40" s="27"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>29</v>
       </c>
@@ -2359,7 +2362,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>0</v>
       </c>
@@ -2386,7 +2389,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>1</v>
       </c>
@@ -2415,7 +2418,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>2</v>
       </c>
@@ -2430,7 +2433,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>3</v>
       </c>
@@ -2459,7 +2462,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>4</v>
       </c>
@@ -2486,7 +2489,7 @@
       <c r="J47" s="3"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>5</v>
       </c>
@@ -2523,7 +2526,7 @@
       </c>
       <c r="J48" s="27"/>
     </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="79"/>
       <c r="D49" s="79"/>
       <c r="E49" s="79"/>
@@ -2533,7 +2536,7 @@
       <c r="I49" s="79"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>31</v>
       </c>
@@ -2550,7 +2553,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>0</v>
       </c>
@@ -2565,7 +2568,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>1</v>
       </c>
@@ -2580,7 +2583,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>2</v>
       </c>
@@ -2595,7 +2598,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>3</v>
       </c>
@@ -2610,7 +2613,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="10"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>4</v>
       </c>
@@ -2625,7 +2628,7 @@
       <c r="J55" s="3"/>
       <c r="K55" s="10"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>5</v>
       </c>
@@ -2662,7 +2665,7 @@
       </c>
       <c r="J56" s="31"/>
     </row>
-    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="79"/>
       <c r="D57" s="79"/>
       <c r="E57" s="79"/>
@@ -2672,7 +2675,7 @@
       <c r="I57" s="79"/>
       <c r="K57" s="10"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>32</v>
       </c>
@@ -2687,7 +2690,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="10"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +2717,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="10"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>1</v>
       </c>
@@ -2741,7 +2744,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="10"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>2</v>
       </c>
@@ -2756,7 +2759,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>3</v>
       </c>
@@ -2783,7 +2786,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="10"/>
     </row>
-    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>4</v>
       </c>
@@ -2810,7 +2813,7 @@
       <c r="J63" s="3"/>
       <c r="K63" s="10"/>
     </row>
-    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>5</v>
       </c>
@@ -2847,7 +2850,7 @@
       </c>
       <c r="J64" s="31"/>
     </row>
-    <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="10"/>
       <c r="C65" s="83"/>
       <c r="D65" s="83"/>
@@ -2859,7 +2862,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="10"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>33</v>
       </c>
@@ -2874,7 +2877,7 @@
       <c r="J66" s="15"/>
       <c r="K66" s="10"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>0</v>
       </c>
@@ -2901,7 +2904,7 @@
       <c r="J67" s="17"/>
       <c r="K67" s="10"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>1</v>
       </c>
@@ -2928,7 +2931,7 @@
       <c r="J68" s="17"/>
       <c r="K68" s="10"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>2</v>
       </c>
@@ -2943,7 +2946,7 @@
       <c r="J69" s="17"/>
       <c r="K69" s="10"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>3</v>
       </c>
@@ -2968,7 +2971,7 @@
       <c r="J70" s="17"/>
       <c r="K70" s="10"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>4</v>
       </c>
@@ -2993,7 +2996,7 @@
       <c r="J71" s="19"/>
       <c r="K71" s="10"/>
     </row>
-    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="27" t="s">
         <v>5</v>
       </c>
@@ -3030,7 +3033,7 @@
       </c>
       <c r="J72" s="31"/>
     </row>
-    <row r="73" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="79"/>
       <c r="D73" s="79"/>
       <c r="E73" s="79"/>
@@ -3040,7 +3043,7 @@
       <c r="I73" s="79"/>
       <c r="K73" s="10"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>34</v>
       </c>
@@ -3055,7 +3058,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="10"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>0</v>
       </c>
@@ -3070,7 +3073,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="10"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>1</v>
       </c>
@@ -3093,7 +3096,7 @@
       </c>
       <c r="K76" s="10"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>2</v>
       </c>
@@ -3108,7 +3111,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="10"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>3</v>
       </c>
@@ -3135,7 +3138,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="10"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>4</v>
       </c>
@@ -3162,7 +3165,7 @@
       <c r="J79" s="3"/>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>5</v>
       </c>
@@ -3199,7 +3202,7 @@
       </c>
       <c r="J80" s="31"/>
     </row>
-    <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="79"/>
       <c r="D81" s="79"/>
       <c r="E81" s="79"/>
@@ -3209,7 +3212,7 @@
       <c r="I81" s="79"/>
       <c r="K81" s="10"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>35</v>
       </c>
@@ -3224,7 +3227,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="10"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>0</v>
       </c>
@@ -3251,7 +3254,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="10"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>1</v>
       </c>
@@ -3278,7 +3281,7 @@
       </c>
       <c r="K84" s="10"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>2</v>
       </c>
@@ -3305,7 +3308,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="10"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>3</v>
       </c>
@@ -3314,15 +3317,25 @@
       </c>
       <c r="C86" s="34"/>
       <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
+      <c r="E86" s="35">
+        <v>4</v>
+      </c>
       <c r="F86" s="35"/>
-      <c r="G86" s="35"/>
-      <c r="H86" s="35"/>
-      <c r="I86" s="36"/>
-      <c r="J86" s="2"/>
+      <c r="G86" s="35">
+        <v>4</v>
+      </c>
+      <c r="H86" s="35">
+        <v>4</v>
+      </c>
+      <c r="I86" s="36">
+        <v>4</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="K86" s="10"/>
     </row>
-    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>4</v>
       </c>
@@ -3339,7 +3352,7 @@
       <c r="J87" s="3"/>
       <c r="K87" s="10"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>5</v>
       </c>
@@ -3356,7 +3369,7 @@
       </c>
       <c r="E88" s="77">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F88" s="77">
         <f t="shared" si="10"/>
@@ -3364,19 +3377,19 @@
       </c>
       <c r="G88" s="77">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H88" s="77">
         <f>SUM(H83:H87)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I88" s="78">
         <f>SUM(I83:I87)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J88" s="31"/>
     </row>
-    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="79"/>
       <c r="D89" s="79"/>
       <c r="E89" s="79"/>
@@ -3386,7 +3399,7 @@
       <c r="I89" s="79"/>
       <c r="K89" s="10"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>36</v>
       </c>
@@ -3401,7 +3414,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="10"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>0</v>
       </c>
@@ -3416,7 +3429,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="10"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>1</v>
       </c>
@@ -3431,7 +3444,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="10"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>2</v>
       </c>
@@ -3446,7 +3459,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="10"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>3</v>
       </c>
@@ -3461,7 +3474,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="10"/>
     </row>
-    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>4</v>
       </c>
@@ -3476,7 +3489,7 @@
       <c r="J95" s="3"/>
       <c r="K95" s="10"/>
     </row>
-    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>5</v>
       </c>
@@ -3513,7 +3526,7 @@
       </c>
       <c r="J96" s="31"/>
     </row>
-    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C97" s="79"/>
       <c r="D97" s="79"/>
       <c r="E97" s="79"/>
@@ -3523,7 +3536,7 @@
       <c r="I97" s="79"/>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>37</v>
       </c>
@@ -3538,7 +3551,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="10"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>0</v>
       </c>
@@ -3553,7 +3566,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="10"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>1</v>
       </c>
@@ -3568,7 +3581,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="10"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>2</v>
       </c>
@@ -3583,7 +3596,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="10"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>3</v>
       </c>
@@ -3598,7 +3611,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="10"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>4</v>
       </c>
@@ -3613,7 +3626,7 @@
       <c r="J103" s="3"/>
       <c r="K103" s="10"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>5</v>
       </c>
@@ -3650,7 +3663,7 @@
       </c>
       <c r="J104" s="27"/>
     </row>
-    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C105" s="79"/>
       <c r="D105" s="79"/>
       <c r="E105" s="79"/>
@@ -3660,7 +3673,7 @@
       <c r="I105" s="79"/>
       <c r="K105" s="10"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>37</v>
       </c>
@@ -3675,7 +3688,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="10"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>0</v>
       </c>
@@ -3690,7 +3703,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="10"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>1</v>
       </c>
@@ -3705,7 +3718,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="10"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>2</v>
       </c>
@@ -3720,7 +3733,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="10"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>3</v>
       </c>
@@ -3735,7 +3748,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>4</v>
       </c>
@@ -3749,7 +3762,7 @@
       <c r="I111" s="81"/>
       <c r="J111" s="3"/>
     </row>
-    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>5</v>
       </c>
@@ -3787,10 +3800,10 @@
       <c r="J112" s="27"/>
       <c r="K112" s="10"/>
     </row>
-    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K113" s="10"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>38</v>
       </c>
@@ -3805,7 +3818,7 @@
       <c r="J114" s="1"/>
       <c r="K114" s="10"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3847,7 @@
       <c r="J115" s="2"/>
       <c r="K115" s="10"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>1</v>
       </c>
@@ -3863,7 +3876,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="10"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>2</v>
       </c>
@@ -3892,7 +3905,7 @@
       <c r="J117" s="2"/>
       <c r="K117" s="10"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>3</v>
       </c>
@@ -3921,7 +3934,7 @@
       <c r="J118" s="2"/>
       <c r="K118" s="10"/>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>4</v>
       </c>
@@ -3949,7 +3962,7 @@
       </c>
       <c r="J119" s="3"/>
     </row>
-    <row r="120" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>5</v>
       </c>
@@ -3987,7 +4000,7 @@
       <c r="J120" s="27"/>
       <c r="K120" s="10"/>
     </row>
-    <row r="121" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="79"/>
       <c r="D121" s="79"/>
       <c r="E121" s="79"/>
@@ -3997,7 +4010,7 @@
       <c r="I121" s="79"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>39</v>
       </c>
@@ -4012,7 +4025,7 @@
       <c r="J122" s="1"/>
       <c r="K122" s="10"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>0</v>
       </c>
@@ -4041,7 +4054,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="10"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>1</v>
       </c>
@@ -4070,7 +4083,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="10"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>2</v>
       </c>
@@ -4099,7 +4112,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="10"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>3</v>
       </c>
@@ -4128,7 +4141,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="10"/>
     </row>
-    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>4</v>
       </c>
@@ -4156,7 +4169,7 @@
       </c>
       <c r="J127" s="3"/>
     </row>
-    <row r="128" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>5</v>
       </c>
@@ -4194,7 +4207,7 @@
       <c r="J128" s="27"/>
       <c r="K128" s="10"/>
     </row>
-    <row r="129" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C129" s="79"/>
       <c r="D129" s="79"/>
       <c r="E129" s="79"/>
@@ -4204,7 +4217,7 @@
       <c r="I129" s="79"/>
       <c r="K129" s="10"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>40</v>
       </c>
@@ -4219,7 +4232,7 @@
       <c r="J130" s="1"/>
       <c r="K130" s="10"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>0</v>
       </c>
@@ -4248,7 +4261,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="10"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>1</v>
       </c>
@@ -4277,7 +4290,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="10"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>2</v>
       </c>
@@ -4306,7 +4319,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="10"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>3</v>
       </c>
@@ -4335,7 +4348,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="10"/>
     </row>
-    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>4</v>
       </c>
@@ -4363,7 +4376,7 @@
       </c>
       <c r="J135" s="3"/>
     </row>
-    <row r="136" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>5</v>
       </c>
@@ -4401,7 +4414,7 @@
       <c r="J136" s="27"/>
       <c r="K136" s="10"/>
     </row>
-    <row r="137" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C137" s="79"/>
       <c r="D137" s="79"/>
       <c r="E137" s="79"/>
@@ -4411,7 +4424,7 @@
       <c r="I137" s="79"/>
       <c r="K137" s="10"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>41</v>
       </c>
@@ -4426,7 +4439,7 @@
       <c r="J138" s="15"/>
       <c r="K138" s="10"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>0</v>
       </c>
@@ -4455,7 +4468,7 @@
       <c r="J139" s="17"/>
       <c r="K139" s="10"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>1</v>
       </c>
@@ -4484,7 +4497,7 @@
       <c r="J140" s="17"/>
       <c r="K140" s="10"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>2</v>
       </c>
@@ -4513,7 +4526,7 @@
       <c r="J141" s="17"/>
       <c r="K141" s="10"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>3</v>
       </c>
@@ -4542,7 +4555,7 @@
       <c r="J142" s="17"/>
       <c r="K142" s="10"/>
     </row>
-    <row r="143" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>4</v>
       </c>
@@ -4570,7 +4583,7 @@
       </c>
       <c r="J143" s="19"/>
     </row>
-    <row r="144" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>5</v>
       </c>
@@ -4608,7 +4621,7 @@
       <c r="J144" s="85"/>
       <c r="K144" s="10"/>
     </row>
-    <row r="145" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="20"/>
       <c r="C145" s="79"/>
       <c r="D145" s="79"/>
@@ -4620,7 +4633,7 @@
       <c r="J145" s="21"/>
       <c r="K145" s="10"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>42</v>
       </c>
@@ -4635,7 +4648,7 @@
       <c r="J146" s="15"/>
       <c r="K146" s="10"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>0</v>
       </c>
@@ -4664,7 +4677,7 @@
       <c r="J147" s="17"/>
       <c r="K147" s="10"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>1</v>
       </c>
@@ -4693,7 +4706,7 @@
       <c r="J148" s="17"/>
       <c r="K148" s="10"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>2</v>
       </c>
@@ -4722,7 +4735,7 @@
       <c r="J149" s="17"/>
       <c r="K149" s="10"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>3</v>
       </c>
@@ -4751,7 +4764,7 @@
       <c r="J150" s="17"/>
       <c r="K150" s="10"/>
     </row>
-    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>4</v>
       </c>
@@ -4779,7 +4792,7 @@
       </c>
       <c r="J151" s="19"/>
     </row>
-    <row r="152" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>5</v>
       </c>
@@ -4817,7 +4830,7 @@
       <c r="J152" s="27"/>
       <c r="K152" s="10"/>
     </row>
-    <row r="153" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C153" s="79"/>
       <c r="D153" s="79"/>
       <c r="E153" s="79"/>
@@ -4827,7 +4840,7 @@
       <c r="I153" s="79"/>
       <c r="K153" s="10"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>43</v>
       </c>
@@ -4842,7 +4855,7 @@
       <c r="J154" s="1"/>
       <c r="K154" s="10"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>0</v>
       </c>
@@ -4871,7 +4884,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="10"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>1</v>
       </c>
@@ -4900,7 +4913,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="10"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>2</v>
       </c>
@@ -4929,7 +4942,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="10"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>3</v>
       </c>
@@ -4958,7 +4971,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="10"/>
     </row>
-    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>4</v>
       </c>
@@ -4986,7 +4999,7 @@
       </c>
       <c r="J159" s="3"/>
     </row>
-    <row r="160" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>5</v>
       </c>
@@ -5024,7 +5037,7 @@
       <c r="J160" s="27"/>
       <c r="K160" s="10"/>
     </row>
-    <row r="161" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C161" s="79"/>
       <c r="D161" s="79"/>
       <c r="E161" s="79"/>
@@ -5034,7 +5047,7 @@
       <c r="I161" s="79"/>
       <c r="K161" s="10"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>44</v>
       </c>
@@ -5049,7 +5062,7 @@
       <c r="J162" s="1"/>
       <c r="K162" s="10"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>0</v>
       </c>
@@ -5078,7 +5091,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="10"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>1</v>
       </c>
@@ -5107,7 +5120,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="10"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>2</v>
       </c>
@@ -5136,7 +5149,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="10"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>3</v>
       </c>
@@ -5165,7 +5178,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="10"/>
     </row>
-    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>4</v>
       </c>
@@ -5193,7 +5206,7 @@
       </c>
       <c r="J167" s="3"/>
     </row>
-    <row r="168" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>5</v>
       </c>
@@ -5231,7 +5244,7 @@
       <c r="J168" s="27"/>
       <c r="K168" s="10"/>
     </row>
-    <row r="169" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C169" s="79"/>
       <c r="D169" s="79"/>
       <c r="E169" s="79"/>
@@ -5241,7 +5254,7 @@
       <c r="I169" s="79"/>
       <c r="K169" s="10"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>10</v>
       </c>
@@ -5256,7 +5269,7 @@
       <c r="J170" s="1"/>
       <c r="K170" s="10"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>0</v>
       </c>
@@ -5285,7 +5298,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="10"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>1</v>
       </c>
@@ -5314,7 +5327,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="10"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>2</v>
       </c>
@@ -5343,7 +5356,7 @@
       <c r="J173" s="2"/>
       <c r="K173" s="10"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>3</v>
       </c>
@@ -5372,7 +5385,7 @@
       <c r="J174" s="2"/>
       <c r="K174" s="10"/>
     </row>
-    <row r="175" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>4</v>
       </c>
@@ -5400,7 +5413,7 @@
       </c>
       <c r="J175" s="3"/>
     </row>
-    <row r="176" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>